<commit_message>
Fixed up OUTPUT() - does not include images anymore - good for SA
</commit_message>
<xml_diff>
--- a/Sensitivity Analysis.xlsx
+++ b/Sensitivity Analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Parameter</t>
   </si>
@@ -31,12 +31,6 @@
     <t>area</t>
   </si>
   <si>
-    <t>rectangle, cross, hook, eight, tee</t>
-  </si>
-  <si>
-    <t>0.04, 1, 2.25, 6.25, 9</t>
-  </si>
-  <si>
     <t>numbFPspecies</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>systematic</t>
   </si>
   <si>
-    <t>120 to 180</t>
-  </si>
-  <si>
     <t>0 to 10</t>
   </si>
   <si>
@@ -185,6 +176,9 @@
   </si>
   <si>
     <t>5 to 50</t>
+  </si>
+  <si>
+    <t>rectangle</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1084,38 +1078,38 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
+      <c r="B3" s="3">
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -1123,24 +1117,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="10">
         <v>150</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>43</v>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -1148,13 +1145,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2">
         <v>9</v>
@@ -1162,13 +1159,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2">
         <v>4</v>
@@ -1176,13 +1173,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2">
         <v>4</v>
@@ -1190,233 +1187,233 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="7">
         <v>100</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" s="7">
         <v>0</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="7">
         <v>100</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" s="7">
         <v>1</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" s="7">
         <v>0.5</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" s="7">
         <v>0.5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="7">
         <v>0.01</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" s="7">
         <v>0.01</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="7">
         <v>0</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="7">
         <v>0.2</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="7">
         <v>0.02</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" s="7">
         <v>0</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" s="7">
         <v>0.05</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="7">
         <v>0.05</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="7">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7">
         <v>0.1</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="7">
         <v>0.1</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="D30" s="2">
         <v>2</v>
@@ -1424,35 +1421,35 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" s="7">
         <v>600</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="7">
         <v>10</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="C33" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D33" s="2">
         <v>2</v>

</xml_diff>